<commit_message>
First increment test (almost) compete
</commit_message>
<xml_diff>
--- a/Actuator tests.xlsx
+++ b/Actuator tests.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\umarasghar\Box\UmarAsghar\Research\3D printing Sensors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msaad\Documents\Saad\Research Projects\Dr. Umer's Project\Reverse-Engineered-Actuator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4727ED11-DD1A-49C5-8619-DA51E4AD973E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1E8EF0-F237-42F2-B0F1-8D8DCC678553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5528F499-BA61-40DE-9B17-253551DE5054}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
   <si>
     <t>Test</t>
   </si>
@@ -56,12 +56,21 @@
   <si>
     <t>Actuator</t>
   </si>
+  <si>
+    <t>40, 39, 39, 40, 41, 42, 42, 43, 44, 45, 46</t>
+  </si>
+  <si>
+    <t>28, 27, 27, 27, 28, 29, 31, 32, 34, 35, 36</t>
+  </si>
+  <si>
+    <t>Raw analogue readings</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +94,14 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -175,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,9 +217,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,24 +541,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB668C0-2F0E-429A-95E8-B8BD84195FA8}">
-  <dimension ref="B2:M42"/>
+  <dimension ref="B2:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -568,15 +605,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" s="8">
         <v>0.5</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="F5" s="9"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -590,7 +631,7 @@
       <c r="L5" s="8"/>
       <c r="M5" s="9"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -611,8 +652,20 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13"/>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -633,8 +686,20 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13"/>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -656,7 +721,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -678,7 +743,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="9"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -700,7 +765,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -722,7 +787,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -744,7 +809,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -766,7 +831,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>10</v>
       </c>
@@ -788,7 +853,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>11</v>
       </c>
@@ -810,7 +875,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>12</v>
       </c>
@@ -1222,6 +1287,9 @@
       <c r="B42" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Resistance calculations added to code and spreadsheet
</commit_message>
<xml_diff>
--- a/Actuator tests.xlsx
+++ b/Actuator tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\msaad\Documents\Saad\Research Projects\Dr. Umer's Project\Reverse-Engineered-Actuator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1E8EF0-F237-42F2-B0F1-8D8DCC678553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7EF0D0-A363-4D80-BED6-2DD863C8D68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5528F499-BA61-40DE-9B17-253551DE5054}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Test</t>
   </si>
@@ -64,13 +64,49 @@
   </si>
   <si>
     <t>Raw analogue readings</t>
+  </si>
+  <si>
+    <t>The analogue readings are mappings of actual voltage into 1024 units</t>
+  </si>
+  <si>
+    <t>Therefore:</t>
+  </si>
+  <si>
+    <t>meaning:</t>
+  </si>
+  <si>
+    <t>for example, lets take readign 40</t>
+  </si>
+  <si>
+    <t>thus:</t>
+  </si>
+  <si>
+    <t>while:</t>
+  </si>
+  <si>
+    <t>using R1 to find current in circuit</t>
+  </si>
+  <si>
+    <t>5Vin/1024 = 4.9mV per unit</t>
+  </si>
+  <si>
+    <t>40*0.0049 = 0.196Vreading</t>
+  </si>
+  <si>
+    <t>*these calculations will be implemented within the code*</t>
+  </si>
+  <si>
+    <t>I = Vr1/R1 = (5-0.196)V/220ohm = 4.804Vr1/220ohm= 0.022A = 22mA</t>
+  </si>
+  <si>
+    <t>R2 = Vreading/I = 0.196V/0.022 = 8.91ohm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +143,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -116,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -188,11 +242,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,13 +326,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB668C0-2F0E-429A-95E8-B8BD84195FA8}">
-  <dimension ref="B2:Z42"/>
+  <dimension ref="B2:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8:R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,24 +683,25 @@
     <col min="5" max="5" width="32.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.44140625" customWidth="1"/>
+    <col min="16" max="18" width="15.77734375" customWidth="1"/>
+    <col min="19" max="20" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-    </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
@@ -604,8 +734,20 @@
       <c r="M4" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O4" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="21"/>
+      <c r="T4" s="21"/>
+      <c r="U4" s="21"/>
+      <c r="V4" s="21"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="21"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B5" s="7">
         <v>1</v>
       </c>
@@ -630,8 +772,22 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B6" s="7">
         <v>2</v>
       </c>
@@ -652,20 +808,24 @@
       <c r="K6" s="8"/>
       <c r="L6" s="8"/>
       <c r="M6" s="9"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-    </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="14"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B7" s="7">
         <v>3</v>
       </c>
@@ -686,20 +846,24 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="9"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-    </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="7">
         <v>4</v>
       </c>
@@ -720,8 +884,22 @@
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
       <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="19"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>5</v>
       </c>
@@ -742,8 +920,20 @@
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="O9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="22"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="7">
         <v>6</v>
       </c>
@@ -765,7 +955,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="9"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B11" s="7">
         <v>7</v>
       </c>
@@ -787,7 +977,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B12" s="7">
         <v>8</v>
       </c>
@@ -809,7 +999,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="9"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B13" s="7">
         <v>9</v>
       </c>
@@ -831,7 +1021,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="9"/>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B14" s="7">
         <v>10</v>
       </c>
@@ -853,7 +1043,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B15" s="7">
         <v>11</v>
       </c>
@@ -875,7 +1065,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B16" s="7">
         <v>12</v>
       </c>
@@ -1287,7 +1477,15 @@
       <c r="B42" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="9">
+    <mergeCell ref="O4:X4"/>
+    <mergeCell ref="O9:X9"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P7:S7"/>
+    <mergeCell ref="T7:V7"/>
+    <mergeCell ref="P8:R8"/>
     <mergeCell ref="B3:F3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>